<commit_message>
changed wording past/presense in 2024, modified downloadable data, fixed typos in ranking
</commit_message>
<xml_diff>
--- a/data/ema.xlsx
+++ b/data/ema.xlsx
@@ -34513,9 +34513,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBD34D3E-3BE5-475B-B4BE-118F41C86765}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90BB3C8A-43EA-4E37-84B4-97C8FB92318A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0263A028-53BD-4CEA-8C00-8563DBFF6CF3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22D5326E-C424-4447-8EB8-3BE46A2AD48D}"/>
 </file>
</xml_diff>

<commit_message>
updated site with updated data and text
</commit_message>
<xml_diff>
--- a/data/ema.xlsx
+++ b/data/ema.xlsx
@@ -34275,8 +34275,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100D6442C570680934CB22BA5BC5A092BF3" ma:contentTypeVersion="14" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="352537810bc3c6c10f651080fe7bf026">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07626311-5b23-4afe-aa20-cc40db419bd4" xmlns:ns3="d74b2904-cc6e-4260-b9ea-005e83d891d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="00128a85c890d0b2da9297bff2aa970a" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D6442C570680934CB22BA5BC5A092BF3" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d8715acdad66b2e285dd96b64bd0916a">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07626311-5b23-4afe-aa20-cc40db419bd4" xmlns:ns3="d74b2904-cc6e-4260-b9ea-005e83d891d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e6541d147a18f301eed2e0ff6941535" ns2:_="" ns3:_="">
     <xsd:import namespace="07626311-5b23-4afe-aa20-cc40db419bd4"/>
     <xsd:import namespace="d74b2904-cc6e-4260-b9ea-005e83d891d2"/>
     <xsd:element name="properties">
@@ -34298,6 +34298,7 @@
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -34328,7 +34329,7 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Bildemerkelapper" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="ff15d7e9-da90-449b-8052-bacb1922583c" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="ff15d7e9-da90-449b-8052-bacb1922583c" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -34362,11 +34363,16 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="22" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d74b2904-cc6e-4260-b9ea-005e83d891d2" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Delt med" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -34385,7 +34391,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Delingsdetaljer" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -34413,8 +34419,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Innholdstype"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Tittel"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -34512,10 +34518,25 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07626311-5b23-4afe-aa20-cc40db419bd4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d74b2904-cc6e-4260-b9ea-005e83d891d2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90BB3C8A-43EA-4E37-84B4-97C8FB92318A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F79991E1-8912-416F-9ADA-42F9DEF024BD}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22D5326E-C424-4447-8EB8-3BE46A2AD48D}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC9DFC18-9278-4F7B-A4E0-41104170B53F}"/>
 </file>
</xml_diff>